<commit_message>
final data cleaning for Bulawayo datasets.
</commit_message>
<xml_diff>
--- a/Project 1 -/Data_files/Cities/Bulawayo/Datafiles/Loan Given Report - Bulawayo Mon Aug 29 2022.xlsx
+++ b/Project 1 -/Data_files/Cities/Bulawayo/Datafiles/Loan Given Report - Bulawayo Mon Aug 29 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faith Kabanda\OneDrive\Documents\Data Analysis Portfolio By Faith Kabanda\Data-Analyst-Portfolio-By-Faith-Kabanda\Project 1 -\Data_files\Cities\Bulawayo\Datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BE5305-FD9E-4743-9DF9-4C9556FA38E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB2E7E-23A2-4289-B1D8-7903A9FD2470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11710" yWindow="2310" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -795,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1568,7 +1568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>